<commit_message>
work on the "main table"
</commit_message>
<xml_diff>
--- a/Main Table-2025-07-03.xlsx
+++ b/Main Table-2025-07-03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\GitHub\Liu2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698AF157-8277-4635-8379-BFBADEDC1469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7569A5BF-925C-4FC2-B6CA-1DAD07BE1306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{877376FE-EA8D-42D1-BF7B-E93F05C56434}"/>
+    <workbookView xWindow="-28920" yWindow="1230" windowWidth="29040" windowHeight="15720" xr2:uid="{877376FE-EA8D-42D1-BF7B-E93F05C56434}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -652,6 +652,18 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">    7 InD signatures that were not found in tumors that we analyzed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4 InD signatures that are artefacts per Koh et al. </t>
+  </si>
+  <si>
+    <t>Example tumor with spectrum dominated by the signature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8 InD signatures that can be reconstructed by combinations of &gt; 1 InsDel singature (Table S8).</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
@@ -669,20 +681,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Signatures that in Koh et al. that were not detected in the current study consist of:</t>
+      <t>The sgnatures in Koh et al. that were not detected in the current study consist of:</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">    7 InD signatures that were not found in tumors that we analyzed. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    4 InD signatures that are artefacts per Koh et al. </t>
-  </si>
-  <si>
-    <t>Example tumor with spectrum dominated by the signature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    8 InD signatures that can be reconstructed by combinations of &gt; 1 InsDel singature (Table S8).</t>
   </si>
 </sst>
 </file>
@@ -790,9 +790,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -822,20 +819,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1154,1205 +1154,1194 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A42" sqref="A42:XFD42"/>
+      <selection pane="bottomRight" activeCell="A52" sqref="A52:I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.06640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="34.46484375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.06640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.46484375" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="14.06640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.46484375" style="2" customWidth="1"/>
     <col min="7" max="7" width="13" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.73046875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23.73046875" style="3" customWidth="1"/>
     <col min="9" max="9" width="18.86328125" style="2" customWidth="1"/>
     <col min="10" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" ht="83.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="83.25">
+      <c r="A1" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <v>0.96</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="14"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="13" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <v>0.96</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="14"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="13" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <v>0.91</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="14"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="13"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="17" customHeight="1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <v>0.99</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="14"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="13"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="14"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="13"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="12" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="12">
         <v>0.97</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="14"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="13"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="12">
         <v>0.94</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="14"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="13"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="12">
         <v>0.97499999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="12">
         <v>0.97</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="12">
         <v>0.94399999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="12">
         <v>0.92</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="13"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="13"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="13"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="12">
         <v>0.99</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="12">
         <v>0.98</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="13"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="12">
         <v>0.99</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="13"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="14"/>
-      <c r="B26" s="10" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="14"/>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="13"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="12">
         <v>0.93</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="14"/>
-      <c r="B30" s="10" t="s">
+      <c r="A30" s="17"/>
+      <c r="B30" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="13"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="11" t="s">
+      <c r="B32" s="13"/>
+      <c r="C32" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="13"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="10"/>
-      <c r="I33" s="13"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="13"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H35" s="10"/>
-      <c r="I35" s="13"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H36" s="10"/>
-      <c r="I36" s="13"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H37" s="10"/>
-      <c r="I37" s="13"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="12"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H38" s="10"/>
-      <c r="I38" s="13"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="13"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="H40" s="10"/>
-      <c r="I40" s="13"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="12"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="14"/>
-      <c r="B41" s="10" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="13"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="12"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G42" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H42" s="13" t="s">
+      <c r="H42" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="I42" s="13">
+      <c r="I42" s="12">
         <v>0.97</v>
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="G43" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H43" s="10"/>
-      <c r="I43" s="13"/>
-    </row>
-    <row r="44" spans="1:9" ht="27">
-      <c r="A44" s="10" t="s">
+      <c r="H43" s="9"/>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="G44" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H44" s="10"/>
-      <c r="I44" s="13"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9" ht="17" customHeight="1">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="H45" s="13" t="s">
+      <c r="H45" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="I45" s="13">
+      <c r="I45" s="12">
         <v>0.93</v>
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="17"/>
-      <c r="B46" s="10" t="s">
+      <c r="A46" s="13"/>
+      <c r="B46" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="13"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="12"/>
     </row>
     <row r="47" spans="1:9">
       <c r="H47" s="1"/>
     </row>
-    <row r="49" spans="1:9" s="5" customFormat="1">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:9" s="4" customFormat="1">
+      <c r="A49" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="16" t="s">
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
+      <c r="A52" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A49:I49"/>
-    <mergeCell ref="A50:I50"/>
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A52:I52"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D12:D13"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
     <mergeCell ref="E6:E8"/>
@@ -2363,17 +2352,28 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="A49:I49"/>
+    <mergeCell ref="A50:I50"/>
+    <mergeCell ref="A51:I51"/>
+    <mergeCell ref="A52:I52"/>
+    <mergeCell ref="G45:G46"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>